<commit_message>
fixed nested vpc stack
</commit_message>
<xml_diff>
--- a/aws-auto-remediate-pci-securityhub/config/AWS Security Hub Benchmarks-Coverage.xlsx
+++ b/aws-auto-remediate-pci-securityhub/config/AWS Security Hub Benchmarks-Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanishk.mahajan\Documents\GitHub-awsmigrations\awstransformationsamples\aws-auto-remediate-pci-securityhub\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A39F183-9EF6-4C72-A089-8101CC83A70A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EF089F-5B05-4751-9DDC-CA66FED77268}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{E65A1D24-E8B5-0C49-B292-C80D18F77D61}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{E65A1D24-E8B5-0C49-B292-C80D18F77D61}"/>
   </bookViews>
   <sheets>
     <sheet name="CIS" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="227">
   <si>
     <t>1.1 – Avoid the use of the "root" account</t>
   </si>
@@ -698,9 +698,6 @@
     <t>Overlap</t>
   </si>
   <si>
-    <t xml:space="preserve">PCI-SSM.1 </t>
-  </si>
-  <si>
     <t>InstanceID in ASFF not found</t>
   </si>
   <si>
@@ -714,6 +711,9 @@
   </si>
   <si>
     <t>NEW ssm document - Redshift is not supported in ASFF</t>
+  </si>
+  <si>
+    <t>new SSM</t>
   </si>
 </sst>
 </file>
@@ -2164,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52ED7434-A76D-4587-91B2-B2075697C5CB}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2313,7 +2313,7 @@
         <v>137</v>
       </c>
       <c r="D15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
@@ -2324,7 +2324,7 @@
         <v>137</v>
       </c>
       <c r="D16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -2405,7 +2405,7 @@
         <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E25" s="2"/>
     </row>
@@ -2417,7 +2417,7 @@
         <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E26" s="30"/>
     </row>
@@ -2440,7 +2440,7 @@
         <v>31</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E28" s="30"/>
     </row>
@@ -2487,7 +2487,7 @@
         <v>31</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2523,8 +2523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE8AEF8-33F4-43D8-8403-98DC4A4ADC2D}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2553,6 +2553,9 @@
       <c r="C2" s="15" t="s">
         <v>31</v>
       </c>
+      <c r="D2" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="23"/>
@@ -2580,11 +2583,11 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="23"/>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="20" t="s">
         <v>188</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>31</v>
+        <v>137</v>
       </c>
       <c r="D5" t="s">
         <v>218</v>
@@ -2644,6 +2647,9 @@
       <c r="C10" s="16" t="s">
         <v>31</v>
       </c>
+      <c r="D10" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B11" s="21" t="s">
@@ -2652,6 +2658,9 @@
       <c r="C11" s="15" t="s">
         <v>31</v>
       </c>
+      <c r="D11" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" s="21" t="s">
@@ -2660,6 +2669,9 @@
       <c r="C12" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D12" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13" s="29" t="s">
@@ -2679,6 +2691,9 @@
       <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D14" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B15" s="14" t="s">
@@ -2769,6 +2784,9 @@
       <c r="C23" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D23" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="26" t="s">
@@ -2799,6 +2817,9 @@
       <c r="C26" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="D26" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="26" t="s">
@@ -2845,14 +2866,14 @@
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="24" t="s">
         <v>214</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.35">
@@ -2892,12 +2913,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3067,15 +3085,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3D5BD93-DB2E-464F-8CF7-2612201A18EA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED75505B-8D7F-4F30-BEE9-E094F3C09792}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5357d50a-c059-4999-b5e6-c73cf26c3e78"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3099,17 +3128,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED75505B-8D7F-4F30-BEE9-E094F3C09792}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3D5BD93-DB2E-464F-8CF7-2612201A18EA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5357d50a-c059-4999-b5e6-c73cf26c3e78"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
redshift and rds updates
</commit_message>
<xml_diff>
--- a/aws-auto-remediate-pci-securityhub/config/AWS Security Hub Benchmarks-Coverage.xlsx
+++ b/aws-auto-remediate-pci-securityhub/config/AWS Security Hub Benchmarks-Coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub-awsmigrations\awstransformationsamples\aws-auto-remediate-pci-securityhub\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698AAD5C-F150-4515-B08B-B6FB365A9886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28787192-AD25-458A-B6AE-441E7D43FC56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E65A1D24-E8B5-0C49-B292-C80D18F77D61}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Foundational Security" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="233">
   <si>
     <t>1.1 – Avoid the use of the "root" account</t>
   </si>
@@ -704,12 +705,6 @@
     <t>Manual - https://aws.amazon.com/premiumsupport/knowledge-center/migrate-amazon-es-domain/</t>
   </si>
   <si>
-    <t>NEW ssm document - Snapshot ID is not in ASFF</t>
-  </si>
-  <si>
-    <t>NEW ssm document - Redshift is not supported in ASFF</t>
-  </si>
-  <si>
     <t>new SSM</t>
   </si>
   <si>
@@ -725,7 +720,19 @@
     <t>TESTED - NEW ssm document</t>
   </si>
   <si>
-    <t>TESTED - SecurityHub Bug - Works if provided with Snapshot ID - NEW ssm document</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW ssm document </t>
+  </si>
+  <si>
+    <t>TESTED - SecurityHub Bug - No snapshotid in finding. Remediation works if provided with Snapshot ID - NEW ssm document</t>
+  </si>
+  <si>
+    <t>TESTED - NEW ssm document (doesn’t look for sg references--remediation steps in pci docs don't require this)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TESTED - NEW ssm document </t>
   </si>
 </sst>
 </file>
@@ -874,7 +881,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -930,6 +937,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2176,18 +2184,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52ED7434-A76D-4587-91B2-B2075697C5CB}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="82.375" customWidth="1"/>
     <col min="3" max="3" width="26.625" customWidth="1"/>
-    <col min="4" max="4" width="21.375" customWidth="1"/>
+    <col min="4" max="4" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="s">
         <v>183</v>
       </c>
@@ -2198,7 +2206,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
         <v>151</v>
       </c>
@@ -2206,10 +2214,10 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>152</v>
       </c>
@@ -2217,7 +2225,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>153</v>
       </c>
@@ -2225,7 +2233,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>154</v>
       </c>
@@ -2233,7 +2241,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>155</v>
       </c>
@@ -2241,7 +2249,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
         <v>156</v>
       </c>
@@ -2249,7 +2257,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>157</v>
       </c>
@@ -2260,7 +2268,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>158</v>
       </c>
@@ -2268,7 +2276,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>159</v>
       </c>
@@ -2276,7 +2284,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>160</v>
       </c>
@@ -2287,7 +2295,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>161</v>
       </c>
@@ -2295,7 +2303,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>162</v>
       </c>
@@ -2303,10 +2311,13 @@
         <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="E13" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>163</v>
       </c>
@@ -2314,10 +2325,10 @@
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
         <v>164</v>
       </c>
@@ -2328,7 +2339,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="20" t="s">
         <v>165</v>
       </c>
@@ -2406,7 +2417,7 @@
         <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2414,10 +2425,10 @@
         <v>174</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E25" s="2"/>
     </row>
@@ -2429,7 +2440,7 @@
         <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="E26" s="30"/>
     </row>
@@ -2441,7 +2452,7 @@
         <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2452,9 +2463,9 @@
         <v>31</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>224</v>
-      </c>
-      <c r="E28" s="30"/>
+        <v>232</v>
+      </c>
+      <c r="E28" s="31"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
@@ -2480,7 +2491,7 @@
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2566,7 +2577,7 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2660,7 +2671,7 @@
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2671,7 +2682,7 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2682,7 +2693,7 @@
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2704,7 +2715,7 @@
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2797,7 +2808,7 @@
         <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -2830,7 +2841,7 @@
         <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -2885,7 +2896,7 @@
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -2925,6 +2936,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B804CAAC924FD246AAC2FBB8E8CC3975" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="574679e58e266fc9ee7cf315443f59a4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5357d50a-c059-4999-b5e6-c73cf26c3e78" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f8548d416c145f84c96b81fd6c9c2574" ns2:_="">
     <xsd:import namespace="5357d50a-c059-4999-b5e6-c73cf26c3e78"/>
@@ -3090,12 +3107,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3106,6 +3117,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED75505B-8D7F-4F30-BEE9-E094F3C09792}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5357d50a-c059-4999-b5e6-c73cf26c3e78"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3A48F9B-AD05-4869-B1CB-AAD745C3926B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3123,22 +3150,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED75505B-8D7F-4F30-BEE9-E094F3C09792}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5357d50a-c059-4999-b5e6-c73cf26c3e78"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3D5BD93-DB2E-464F-8CF7-2612201A18EA}">
   <ds:schemaRefs>

</xml_diff>